<commit_message>
Add total speed datum
</commit_message>
<xml_diff>
--- a/sw/speed.xlsx
+++ b/sw/speed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Fetch</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Interval (ns)</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +391,7 @@
     <col min="1" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +407,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -424,8 +430,11 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -434,7 +443,7 @@
         <v>400</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:F3" si="0">1/C2*1000</f>
+        <f t="shared" ref="C3:G3" si="0">1/C2*1000</f>
         <v>666.66666666666663</v>
       </c>
       <c r="D3" s="1">
@@ -448,6 +457,10 @@
       <c r="F3" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>